<commit_message>
Updated site info and param list
</commit_message>
<xml_diff>
--- a/output/for_plots/param_list.xlsx
+++ b/output/for_plots/param_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kashifmahmud/IU/Work/All_analyses/semi-arid_sites/output/for_plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F455D5-922F-1340-9A7F-739536EF8501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8057BCB7-E76A-9246-B569-4FE5FE84B4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20760" yWindow="460" windowWidth="15760" windowHeight="18520" xr2:uid="{EB883CC8-6C5C-AE42-9F98-11BF953A935F}"/>
+    <workbookView xWindow="17840" yWindow="500" windowWidth="15760" windowHeight="18520" xr2:uid="{EB883CC8-6C5C-AE42-9F98-11BF953A935F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>VMAX_OFFSET</t>
   </si>
   <si>
-    <t>Post GPP</t>
-  </si>
-  <si>
     <t>fpseudo</t>
   </si>
   <si>
@@ -309,6 +306,9 @@
   </si>
   <si>
     <t>Param_type</t>
+  </si>
+  <si>
+    <t>Post C uptake</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EFA0D8-D08C-6545-80AC-382E36BCA8F0}">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,10 +674,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
         <v>90</v>
-      </c>
-      <c r="B1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -709,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -717,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -725,7 +725,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -733,7 +733,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -741,7 +741,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -749,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -757,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -765,7 +765,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -781,15 +781,15 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -797,583 +797,583 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>